<commit_message>
add Same As + Persons sheets to Excel template, add T-077 import-excel task
Panel review identified missing Same As sheet (P0, critical for merge
viability) and Persons sheet (covers all 7 OMTS node types). Updated
README sheet with entity deduplication and person node privacy sections.
Added T-077 to backlog for implementing the import-excel CLI command.
</commit_message>
<xml_diff>
--- a/tests/fixtures/excel/omts-import-example.xlsx
+++ b/tests/fixtures/excel/omts-import-example.xlsx
@@ -13,20 +13,24 @@
     <sheet name="Facilities" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="Goods" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="Attestations" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Consignments" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="Supply Relationships" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="Corporate Structure" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="Identifiers" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="Persons" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Consignments" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Supply Relationships" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="Corporate Structure" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="Same As" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="Identifiers" sheetId="12" state="visible" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Organizations'!$A$1:$O$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Facilities'!$A$1:$I$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Goods'!$A$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Attestations'!$A$1:$N$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Consignments'!$A$1:$K$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Supply Relationships'!$A$1:$O$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Corporate Structure'!$A$1:$J$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'Identifiers'!$A$1:$H$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Persons'!$A$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Consignments'!$A$1:$K$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Supply Relationships'!$A$1:$O$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'Corporate Structure'!$A$1:$J$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'Same As'!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'Identifiers'!$A$1:$H$1</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -487,7 +491,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B46"/>
+  <dimension ref="A1:B58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -590,103 +594,103 @@
     <row r="11">
       <c r="A11" s="2" t="inlineStr">
         <is>
-          <t>Attestations</t>
+          <t>Persons</t>
         </is>
       </c>
       <c r="B11" s="2" t="inlineStr">
         <is>
-          <t>Certifications, audits, due diligence statements.</t>
+          <t>Beneficial owners, key individuals (sensitivity: confidential by default).</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>Consignments</t>
+          <t>Attestations</t>
         </is>
       </c>
       <c r="B12" s="2" t="inlineStr">
         <is>
-          <t>Batches, lots, shipments (optional, for CBAM/EUDR).</t>
+          <t>Certifications, audits, due diligence statements.</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>Supply Relationships</t>
+          <t>Consignments</t>
         </is>
       </c>
       <c r="B13" s="2" t="inlineStr">
         <is>
-          <t>Supply, subcontracting, tolling, distribution edges.</t>
+          <t>Batches, lots, shipments (optional, for CBAM/EUDR).</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>Corporate Structure</t>
+          <t>Supply Relationships</t>
         </is>
       </c>
       <c r="B14" s="2" t="inlineStr">
         <is>
-          <t>Ownership, legal parentage, operational control edges.</t>
+          <t>Supply, subcontracting, tolling, distribution edges.</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="inlineStr">
         <is>
+          <t>Corporate Structure</t>
+        </is>
+      </c>
+      <c r="B15" s="2" t="inlineStr">
+        <is>
+          <t>Ownership, legal parentage, operational control edges.</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="inlineStr">
+        <is>
+          <t>Same As</t>
+        </is>
+      </c>
+      <c r="B16" s="2" t="inlineStr">
+        <is>
+          <t>Entity deduplication: link nodes that represent the same real-world entity.</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="inlineStr">
+        <is>
           <t>Identifiers</t>
         </is>
       </c>
-      <c r="B15" s="2" t="inlineStr">
+      <c r="B17" s="2" t="inlineStr">
         <is>
           <t>Advanced: additional identifiers beyond the common columns.</t>
         </is>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="2" t="inlineStr"/>
-      <c r="B16" s="2" t="inlineStr"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="4" t="inlineStr">
+    <row r="18">
+      <c r="A18" s="2" t="inlineStr"/>
+      <c r="B18" s="2" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="4" t="inlineStr">
         <is>
           <t>REQUIRED FIELDS</t>
         </is>
       </c>
-      <c r="B17" s="2" t="inlineStr"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="2" t="inlineStr">
-        <is>
-          <t>Organizations</t>
-        </is>
-      </c>
-      <c r="B18" s="2" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="2" t="inlineStr">
-        <is>
-          <t>Facilities</t>
-        </is>
-      </c>
-      <c r="B19" s="2" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
+      <c r="B19" s="2" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" s="2" t="inlineStr">
         <is>
-          <t>Goods</t>
+          <t>Organizations</t>
         </is>
       </c>
       <c r="B20" s="2" t="inlineStr">
@@ -698,71 +702,79 @@
     <row r="21">
       <c r="A21" s="2" t="inlineStr">
         <is>
-          <t>Attestations</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="B21" s="2" t="inlineStr">
         <is>
-          <t>name, attestation_type, valid_from</t>
+          <t>name</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>Supply Relationships</t>
+          <t>Goods</t>
         </is>
       </c>
       <c r="B22" s="2" t="inlineStr">
         <is>
-          <t>type, supplier_id, buyer_id, valid_from</t>
+          <t>name</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="inlineStr">
         <is>
+          <t>Attestations</t>
+        </is>
+      </c>
+      <c r="B23" s="2" t="inlineStr">
+        <is>
+          <t>name, attestation_type, valid_from</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="inlineStr">
+        <is>
+          <t>Supply Relationships</t>
+        </is>
+      </c>
+      <c r="B24" s="2" t="inlineStr">
+        <is>
+          <t>type, supplier_id, buyer_id, valid_from</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="inlineStr">
+        <is>
           <t>Corporate Structure</t>
         </is>
       </c>
-      <c r="B23" s="2" t="inlineStr">
+      <c r="B25" s="2" t="inlineStr">
         <is>
           <t>type, subsidiary_id, parent_id, valid_from</t>
         </is>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" s="2" t="inlineStr"/>
-      <c r="B24" s="2" t="inlineStr"/>
-    </row>
-    <row r="25">
-      <c r="A25" s="4" t="inlineStr">
+    <row r="26">
+      <c r="A26" s="2" t="inlineStr"/>
+      <c r="B26" s="2" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="4" t="inlineStr">
         <is>
           <t>AUTO-GENERATED FIELDS</t>
         </is>
       </c>
-      <c r="B25" s="2" t="inlineStr"/>
-    </row>
-    <row r="26">
-      <c r="A26" s="2" t="inlineStr">
+      <c r="B27" s="2" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="inlineStr">
         <is>
           <t>The import command will auto-generate:</t>
-        </is>
-      </c>
-      <c r="B26" s="2" t="inlineStr"/>
-    </row>
-    <row r="27">
-      <c r="A27" s="3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  - file_salt (cryptographic random)</t>
-        </is>
-      </c>
-      <c r="B27" s="2" t="inlineStr"/>
-    </row>
-    <row r="28">
-      <c r="A28" s="3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  - node/edge IDs (if left blank)</t>
         </is>
       </c>
       <c r="B28" s="2" t="inlineStr"/>
@@ -770,7 +782,7 @@
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - boundary_ref nodes (if disclosure_scope set)</t>
+          <t xml:space="preserve">  - file_salt (cryptographic random)</t>
         </is>
       </c>
       <c r="B29" s="2" t="inlineStr"/>
@@ -778,35 +790,35 @@
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
         <is>
+          <t xml:space="preserve">  - node/edge IDs (if left blank)</t>
+        </is>
+      </c>
+      <c r="B30" s="2" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  - boundary_ref nodes (if disclosure_scope set)</t>
+        </is>
+      </c>
+      <c r="B31" s="2" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="3" t="inlineStr">
+        <is>
           <t xml:space="preserve">  - sensitivity defaults per SPEC-004</t>
         </is>
       </c>
-      <c r="B30" s="2" t="inlineStr"/>
-    </row>
-    <row r="31">
-      <c r="A31" s="2" t="inlineStr"/>
-      <c r="B31" s="2" t="inlineStr"/>
-    </row>
-    <row r="32">
-      <c r="A32" s="4" t="inlineStr">
+      <c r="B32" s="2" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="2" t="inlineStr"/>
+      <c r="B33" s="2" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="4" t="inlineStr">
         <is>
           <t>IDENTIFIER COLUMNS</t>
-        </is>
-      </c>
-      <c r="B32" s="2" t="inlineStr"/>
-    </row>
-    <row r="33">
-      <c r="A33" s="2" t="inlineStr">
-        <is>
-          <t>Common identifiers have dedicated columns on the Organizations sheet:</t>
-        </is>
-      </c>
-      <c r="B33" s="2" t="inlineStr"/>
-    </row>
-    <row r="34">
-      <c r="A34" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  lei          - Legal Entity Identifier (20-char, validated)</t>
         </is>
       </c>
       <c r="B34" s="2" t="inlineStr"/>
@@ -814,7 +826,7 @@
     <row r="35">
       <c r="A35" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">  duns         - DUNS Number (9-digit, validated)</t>
+          <t>Common identifiers have dedicated columns on the Organizations sheet:</t>
         </is>
       </c>
       <c r="B35" s="2" t="inlineStr"/>
@@ -822,7 +834,7 @@
     <row r="36">
       <c r="A36" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">  nat_reg_*    - National registry number + GLEIF RA authority code</t>
+          <t xml:space="preserve">  lei          - Legal Entity Identifier (20-char, validated)</t>
         </is>
       </c>
       <c r="B36" s="2" t="inlineStr"/>
@@ -830,7 +842,7 @@
     <row r="37">
       <c r="A37" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">  vat_*        - VAT/tax ID + ISO 3166-1 alpha-2 country code</t>
+          <t xml:space="preserve">  duns         - DUNS Number (9-digit, validated)</t>
         </is>
       </c>
       <c r="B37" s="2" t="inlineStr"/>
@@ -838,7 +850,7 @@
     <row r="38">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">  internal_*   - Internal system ID + system name</t>
+          <t xml:space="preserve">  nat_reg_*    - National registry number + GLEIF RA authority code</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr"/>
@@ -846,58 +858,146 @@
     <row r="39">
       <c r="A39" s="2" t="inlineStr">
         <is>
+          <t xml:space="preserve">  vat_*        - VAT/tax ID + ISO 3166-1 alpha-2 country code</t>
+        </is>
+      </c>
+      <c r="B39" s="2" t="inlineStr"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  internal_*   - Internal system ID + system name</t>
+        </is>
+      </c>
+      <c r="B40" s="2" t="inlineStr"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="2" t="inlineStr">
+        <is>
           <t>For multiple IDs of the same scheme, use the Identifiers sheet.</t>
         </is>
       </c>
-      <c r="B39" s="2" t="inlineStr"/>
-    </row>
-    <row r="40">
-      <c r="A40" s="2" t="inlineStr"/>
-      <c r="B40" s="2" t="inlineStr"/>
-    </row>
-    <row r="41">
-      <c r="A41" s="4" t="inlineStr">
+      <c r="B41" s="2" t="inlineStr"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="2" t="inlineStr"/>
+      <c r="B42" s="2" t="inlineStr"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="4" t="inlineStr">
         <is>
           <t>EDGE DIRECTION</t>
         </is>
       </c>
-      <c r="B41" s="2" t="inlineStr"/>
-    </row>
-    <row r="42">
-      <c r="A42" s="2" t="inlineStr">
+      <c r="B43" s="2" t="inlineStr"/>
+    </row>
+    <row r="44">
+      <c r="A44" s="2" t="inlineStr">
         <is>
           <t>Supply Relationships: supplier_id = who supplies, buyer_id = who buys</t>
         </is>
       </c>
-      <c r="B42" s="2" t="inlineStr"/>
-    </row>
-    <row r="43">
-      <c r="A43" s="2" t="inlineStr">
+      <c r="B44" s="2" t="inlineStr"/>
+    </row>
+    <row r="45">
+      <c r="A45" s="2" t="inlineStr">
         <is>
           <t>Corporate Structure: subsidiary_id = child entity, parent_id = parent entity</t>
         </is>
       </c>
-      <c r="B43" s="2" t="inlineStr"/>
-    </row>
-    <row r="44">
-      <c r="A44" s="2" t="inlineStr"/>
-      <c r="B44" s="2" t="inlineStr"/>
-    </row>
-    <row r="45">
-      <c r="A45" s="4" t="inlineStr">
+      <c r="B45" s="2" t="inlineStr"/>
+    </row>
+    <row r="46">
+      <c r="A46" s="2" t="inlineStr"/>
+      <c r="B46" s="2" t="inlineStr"/>
+    </row>
+    <row r="47">
+      <c r="A47" s="4" t="inlineStr">
+        <is>
+          <t>ENTITY DEDUPLICATION</t>
+        </is>
+      </c>
+      <c r="B47" s="2" t="inlineStr"/>
+    </row>
+    <row r="48">
+      <c r="A48" s="2" t="inlineStr">
+        <is>
+          <t>Use the Same As sheet to link nodes that represent the same real-world entity</t>
+        </is>
+      </c>
+      <c r="B48" s="2" t="inlineStr"/>
+    </row>
+    <row r="49">
+      <c r="A49" s="2" t="inlineStr">
+        <is>
+          <t>but appear as separate rows (e.g., same company under different names/IDs).</t>
+        </is>
+      </c>
+      <c r="B49" s="2" t="inlineStr"/>
+    </row>
+    <row r="50">
+      <c r="A50" s="2" t="inlineStr">
+        <is>
+          <t>The import command uses these to generate same_as edges for merge operations.</t>
+        </is>
+      </c>
+      <c r="B50" s="2" t="inlineStr"/>
+    </row>
+    <row r="51">
+      <c r="A51" s="2" t="inlineStr"/>
+      <c r="B51" s="2" t="inlineStr"/>
+    </row>
+    <row r="52">
+      <c r="A52" s="4" t="inlineStr">
+        <is>
+          <t>PERSON NODE PRIVACY</t>
+        </is>
+      </c>
+      <c r="B52" s="2" t="inlineStr"/>
+    </row>
+    <row r="53">
+      <c r="A53" s="2" t="inlineStr">
+        <is>
+          <t>Person nodes default to confidential sensitivity (SPEC-004).</t>
+        </is>
+      </c>
+      <c r="B53" s="2" t="inlineStr"/>
+    </row>
+    <row r="54">
+      <c r="A54" s="2" t="inlineStr">
+        <is>
+          <t>If disclosure_scope is 'public', the import command will reject the file</t>
+        </is>
+      </c>
+      <c r="B54" s="2" t="inlineStr"/>
+    </row>
+    <row r="55">
+      <c r="A55" s="2" t="inlineStr">
+        <is>
+          <t>if any person nodes are present.</t>
+        </is>
+      </c>
+      <c r="B55" s="2" t="inlineStr"/>
+    </row>
+    <row r="56">
+      <c r="A56" s="2" t="inlineStr"/>
+      <c r="B56" s="2" t="inlineStr"/>
+    </row>
+    <row r="57">
+      <c r="A57" s="4" t="inlineStr">
         <is>
           <t>SPEC VERSION</t>
         </is>
       </c>
-      <c r="B45" s="2" t="inlineStr"/>
-    </row>
-    <row r="46">
-      <c r="A46" s="2" t="inlineStr">
+      <c r="B57" s="2" t="inlineStr"/>
+    </row>
+    <row r="58">
+      <c r="A58" s="2" t="inlineStr">
         <is>
           <t>This template targets OMTS spec version 0.1.0</t>
         </is>
       </c>
-      <c r="B46" s="2" t="inlineStr"/>
+      <c r="B58" s="2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -905,6 +1005,187 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="14" customWidth="1" min="1" max="1"/>
+    <col width="24" customWidth="1" min="2" max="2"/>
+    <col width="18" customWidth="1" min="3" max="3"/>
+    <col width="18" customWidth="1" min="4" max="4"/>
+    <col width="14" customWidth="1" min="5" max="5"/>
+    <col width="14" customWidth="1" min="6" max="6"/>
+    <col width="14" customWidth="1" min="7" max="7"/>
+    <col width="10" customWidth="1" min="8" max="8"/>
+    <col width="26" customWidth="1" min="9" max="9"/>
+    <col width="22" customWidth="1" min="10" max="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="30" customHeight="1">
+      <c r="A1" s="9" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" s="9" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="C1" s="9" t="inlineStr">
+        <is>
+          <t>subsidiary_id</t>
+        </is>
+      </c>
+      <c r="D1" s="9" t="inlineStr">
+        <is>
+          <t>parent_id</t>
+        </is>
+      </c>
+      <c r="E1" s="9" t="inlineStr">
+        <is>
+          <t>valid_from</t>
+        </is>
+      </c>
+      <c r="F1" s="9" t="inlineStr">
+        <is>
+          <t>valid_to</t>
+        </is>
+      </c>
+      <c r="G1" s="9" t="inlineStr">
+        <is>
+          <t>percentage</t>
+        </is>
+      </c>
+      <c r="H1" s="9" t="inlineStr">
+        <is>
+          <t>direct</t>
+        </is>
+      </c>
+      <c r="I1" s="9" t="inlineStr">
+        <is>
+          <t>control_type</t>
+        </is>
+      </c>
+      <c r="J1" s="9" t="inlineStr">
+        <is>
+          <t>consolidation_basis</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>edge-004</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>ownership</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>org-acme</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>org-bolt</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2019-04-01</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:J1"/>
+  <dataValidations count="4">
+    <dataValidation sqref="B2:B10000" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" errorTitle="Invalid value" error="Must be one of: ownership, legal_parentage, operational_control, beneficial_ownership" promptTitle="Edge Type" prompt="Type of corporate relationship" type="list">
+      <formula1>"ownership,legal_parentage,operational_control,beneficial_ownership"</formula1>
+    </dataValidation>
+    <dataValidation sqref="H2:H10000" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" errorTitle="Invalid value" error="Must be one of: TRUE, FALSE" promptTitle="Direct" prompt="Direct or indirect relationship" type="list">
+      <formula1>"TRUE,FALSE"</formula1>
+    </dataValidation>
+    <dataValidation sqref="I2:I10000" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" errorTitle="Invalid value" error="Must be one of: franchise, management, tolling, licensed_manufacturing, other, voting_rights, capital, other_means, senior_management" promptTitle="Control Type" prompt="For operational_control or beneficial_ownership" type="list">
+      <formula1>"franchise,management,tolling,licensed_manufacturing,other,voting_rights,capital,other_means,senior_management"</formula1>
+    </dataValidation>
+    <dataValidation sqref="J2:J10000" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" errorTitle="Invalid value" error="Must be one of: ifrs10, us_gaap_asc810, other, unknown" promptTitle="Consolidation Basis" prompt="For legal_parentage only" type="list">
+      <formula1>"ifrs10,us_gaap_asc810,other,unknown"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="14" customWidth="1" min="3" max="3"/>
+    <col width="40" customWidth="1" min="4" max="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="30" customHeight="1">
+      <c r="A1" s="9" t="inlineStr">
+        <is>
+          <t>entity_a</t>
+        </is>
+      </c>
+      <c r="B1" s="9" t="inlineStr">
+        <is>
+          <t>entity_b</t>
+        </is>
+      </c>
+      <c r="C1" s="9" t="inlineStr">
+        <is>
+          <t>confidence</t>
+        </is>
+      </c>
+      <c r="D1" s="9" t="inlineStr">
+        <is>
+          <t>basis</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:D1"/>
+  <dataValidations count="1">
+    <dataValidation sqref="C2:C10000" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" errorTitle="Invalid value" error="Must be one of: definite, probable, possible" promptTitle="Confidence" prompt="Confidence level of the equivalence assertion" type="list">
+      <formula1>"definite,probable,possible"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1806,6 +2087,60 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="18" customWidth="1" min="1" max="1"/>
+    <col width="30" customWidth="1" min="2" max="2"/>
+    <col width="14" customWidth="1" min="3" max="3"/>
+    <col width="20" customWidth="1" min="4" max="4"/>
+    <col width="14" customWidth="1" min="5" max="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="30" customHeight="1">
+      <c r="A1" s="9" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" s="9" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" s="9" t="inlineStr">
+        <is>
+          <t>jurisdiction</t>
+        </is>
+      </c>
+      <c r="D1" s="9" t="inlineStr">
+        <is>
+          <t>role</t>
+        </is>
+      </c>
+      <c r="E1" s="9" t="inlineStr">
+        <is>
+          <t>nationality</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:E1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1895,7 +2230,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2104,132 +2439,4 @@
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:J2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="14" customWidth="1" min="1" max="1"/>
-    <col width="24" customWidth="1" min="2" max="2"/>
-    <col width="18" customWidth="1" min="3" max="3"/>
-    <col width="18" customWidth="1" min="4" max="4"/>
-    <col width="14" customWidth="1" min="5" max="5"/>
-    <col width="14" customWidth="1" min="6" max="6"/>
-    <col width="14" customWidth="1" min="7" max="7"/>
-    <col width="10" customWidth="1" min="8" max="8"/>
-    <col width="26" customWidth="1" min="9" max="9"/>
-    <col width="22" customWidth="1" min="10" max="10"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="30" customHeight="1">
-      <c r="A1" s="9" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" s="9" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="C1" s="9" t="inlineStr">
-        <is>
-          <t>subsidiary_id</t>
-        </is>
-      </c>
-      <c r="D1" s="9" t="inlineStr">
-        <is>
-          <t>parent_id</t>
-        </is>
-      </c>
-      <c r="E1" s="9" t="inlineStr">
-        <is>
-          <t>valid_from</t>
-        </is>
-      </c>
-      <c r="F1" s="9" t="inlineStr">
-        <is>
-          <t>valid_to</t>
-        </is>
-      </c>
-      <c r="G1" s="9" t="inlineStr">
-        <is>
-          <t>percentage</t>
-        </is>
-      </c>
-      <c r="H1" s="9" t="inlineStr">
-        <is>
-          <t>direct</t>
-        </is>
-      </c>
-      <c r="I1" s="9" t="inlineStr">
-        <is>
-          <t>control_type</t>
-        </is>
-      </c>
-      <c r="J1" s="9" t="inlineStr">
-        <is>
-          <t>consolidation_basis</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>edge-004</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>ownership</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>org-acme</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>org-bolt</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>2019-04-01</t>
-        </is>
-      </c>
-      <c r="G2" t="n">
-        <v>51</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:J1"/>
-  <dataValidations count="4">
-    <dataValidation sqref="B2:B10000" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" errorTitle="Invalid value" error="Must be one of: ownership, legal_parentage, operational_control, beneficial_ownership" promptTitle="Edge Type" prompt="Type of corporate relationship" type="list">
-      <formula1>"ownership,legal_parentage,operational_control,beneficial_ownership"</formula1>
-    </dataValidation>
-    <dataValidation sqref="H2:H10000" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" errorTitle="Invalid value" error="Must be one of: TRUE, FALSE" promptTitle="Direct" prompt="Direct or indirect relationship" type="list">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation sqref="I2:I10000" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" errorTitle="Invalid value" error="Must be one of: franchise, management, tolling, licensed_manufacturing, other, voting_rights, capital, other_means, senior_management" promptTitle="Control Type" prompt="For operational_control or beneficial_ownership" type="list">
-      <formula1>"franchise,management,tolling,licensed_manufacturing,other,voting_rights,capital,other_means,senior_management"</formula1>
-    </dataValidation>
-    <dataValidation sqref="J2:J10000" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" errorTitle="Invalid value" error="Must be one of: ifrs10, us_gaap_asc810, other, unknown" promptTitle="Consolidation Basis" prompt="For legal_parentage only" type="list">
-      <formula1>"ifrs10,us_gaap_asc810,other,unknown"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>